<commit_message>
SUCCESS: build base API connect with Database
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\dung\UET-VNU\nam_3\Phát triển ứng dụng web - Lê Đình Thanh\BaiTap\BTL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\dung\UET-VNU\nam_3\Phát triển ứng dụng web - Lê Đình Thanh\BaiTap\BTL\Git\web-productmove\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="108">
   <si>
     <t>Cơ sở sản xuất</t>
   </si>
@@ -226,18 +226,12 @@
     <t>bornDate</t>
   </si>
   <si>
-    <t>insuranceTime</t>
-  </si>
-  <si>
     <t>agentID</t>
   </si>
   <si>
     <t>startDate</t>
   </si>
   <si>
-    <t>insuranceEndDate</t>
-  </si>
-  <si>
     <t>workplaceID</t>
   </si>
   <si>
@@ -268,12 +262,6 @@
     <t>kết quả</t>
   </si>
   <si>
-    <t>success</t>
-  </si>
-  <si>
-    <t>failure</t>
-  </si>
-  <si>
     <t>roleKey</t>
   </si>
   <si>
@@ -301,9 +289,6 @@
     <t>products</t>
   </si>
   <si>
-    <t>factorys</t>
-  </si>
-  <si>
     <t>agents</t>
   </si>
   <si>
@@ -317,16 +302,70 @@
   </si>
   <si>
     <t>error_reports</t>
+  </si>
+  <si>
+    <t>SUCCESS</t>
+  </si>
+  <si>
+    <t>FAILURE</t>
+  </si>
+  <si>
+    <t>factories</t>
+  </si>
+  <si>
+    <t>errorReportsID</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>R5</t>
+  </si>
+  <si>
+    <t>Customer</t>
+  </si>
+  <si>
+    <t>endDate</t>
+  </si>
+  <si>
+    <t>thành công</t>
+  </si>
+  <si>
+    <t>thất bại</t>
+  </si>
+  <si>
+    <t>màu vàng</t>
+  </si>
+  <si>
+    <t>thêm chức năng sắp xếp</t>
+  </si>
+  <si>
+    <t>cập nhật thay đổi</t>
+  </si>
+  <si>
+    <t>thêm chức năng tìm kiếm theo tên sản phẩm</t>
+  </si>
+  <si>
+    <t>insuranceTermEndDate</t>
+  </si>
+  <si>
+    <t>màu xanh</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -347,7 +386,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -364,13 +403,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -651,28 +692,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N13"/>
+  <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -683,199 +723,217 @@
       <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="O1" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O2" t="s">
+        <v>54</v>
+      </c>
+      <c r="P2" t="s">
         <v>82</v>
       </c>
-      <c r="N1" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="M2" t="s">
-        <v>54</v>
-      </c>
-      <c r="N2" t="s">
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F3" t="s">
+        <v>78</v>
+      </c>
+      <c r="G3" t="s">
+        <v>68</v>
+      </c>
+      <c r="H3" t="s">
+        <v>72</v>
+      </c>
+      <c r="O3" t="s">
+        <v>55</v>
+      </c>
+      <c r="P3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" t="s">
+        <v>59</v>
+      </c>
+      <c r="O4" t="s">
+        <v>56</v>
+      </c>
+      <c r="P4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B5" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="C5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G5" t="s">
+        <v>62</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="O5" t="s">
+        <v>57</v>
+      </c>
+      <c r="P5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E6" t="s">
+        <v>59</v>
+      </c>
+      <c r="O6" t="s">
+        <v>97</v>
+      </c>
+      <c r="P6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7" t="s">
+        <v>59</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
         <v>88</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C8" t="s">
         <v>60</v>
       </c>
-      <c r="C3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D3" t="s">
-        <v>45</v>
-      </c>
-      <c r="E3" t="s">
-        <v>82</v>
-      </c>
-      <c r="F3" t="s">
-        <v>70</v>
-      </c>
-      <c r="G3" t="s">
-        <v>74</v>
-      </c>
-      <c r="M3" t="s">
-        <v>55</v>
-      </c>
-      <c r="N3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>89</v>
-      </c>
-      <c r="B4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="D8" t="s">
         <v>58</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E8" t="s">
         <v>59</v>
       </c>
-      <c r="M4" t="s">
-        <v>56</v>
-      </c>
-      <c r="N4" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>90</v>
-      </c>
-      <c r="B5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C5" t="s">
-        <v>58</v>
-      </c>
-      <c r="D5" t="s">
-        <v>65</v>
-      </c>
-      <c r="E5" t="s">
-        <v>61</v>
-      </c>
-      <c r="F5" t="s">
-        <v>62</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="M5" t="s">
-        <v>57</v>
-      </c>
-      <c r="N5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>91</v>
-      </c>
-      <c r="B6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="O8" t="s">
         <v>92</v>
       </c>
-      <c r="B7" t="s">
-        <v>60</v>
-      </c>
-      <c r="C7" t="s">
-        <v>58</v>
-      </c>
-      <c r="D7" t="s">
-        <v>59</v>
-      </c>
-      <c r="M7" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="N7" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="P8" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N9" t="s">
         <v>93</v>
       </c>
-      <c r="B8" t="s">
-        <v>60</v>
-      </c>
-      <c r="C8" t="s">
-        <v>58</v>
-      </c>
-      <c r="D8" t="s">
-        <v>59</v>
-      </c>
-      <c r="M8" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="M9" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O9" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C11" t="s">
         <v>3</v>
       </c>
       <c r="D11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E11" t="s">
         <v>64</v>
       </c>
       <c r="F11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G11" t="s">
-        <v>67</v>
-      </c>
-      <c r="H11" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C12" t="s">
         <v>3</v>
@@ -883,25 +941,28 @@
       <c r="D12" t="s">
         <v>64</v>
       </c>
-      <c r="E12" t="s">
-        <v>68</v>
+      <c r="E12" s="5" t="s">
+        <v>95</v>
       </c>
       <c r="F12" t="s">
-        <v>66</v>
-      </c>
-      <c r="G12" t="s">
-        <v>78</v>
+        <v>67</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>99</v>
       </c>
       <c r="H12" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+      <c r="I12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C13" t="s">
         <v>3</v>
@@ -913,7 +974,23 @@
         <v>64</v>
       </c>
       <c r="F13" t="s">
-        <v>75</v>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>102</v>
+      </c>
+      <c r="B15" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>107</v>
+      </c>
+      <c r="B16" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>